<commit_message>
push login and register template
</commit_message>
<xml_diff>
--- a/references/Dating.xlsx
+++ b/references/Dating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wodah\Documents\.Woda\Projects\Dating\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D44E595-3469-47BC-A664-050C1F9ADFDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50979C5D-B583-46F2-BF56-5CA1976E0731}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="825" windowWidth="20610" windowHeight="14355" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
+    <workbookView xWindow="2445" yWindow="825" windowWidth="20610" windowHeight="14355" activeTab="1" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="171">
   <si>
     <t>Questionaire</t>
   </si>
@@ -181,6 +181,12 @@
     <t>Parameters</t>
   </si>
   <si>
+    <t>login Name</t>
+  </si>
+  <si>
+    <t>Screen Name</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
@@ -262,6 +268,15 @@
     <t>various</t>
   </si>
   <si>
+    <t>(check availability)</t>
+  </si>
+  <si>
+    <t>Screen Names</t>
+  </si>
+  <si>
+    <t>availability</t>
+  </si>
+  <si>
     <t>question 1</t>
   </si>
   <si>
@@ -448,6 +463,9 @@
     <t>email</t>
   </si>
   <si>
+    <t>password</t>
+  </si>
+  <si>
     <t xml:space="preserve">login Name </t>
   </si>
   <si>
@@ -530,36 +548,6 @@
   </si>
   <si>
     <t>Alexander Marzullo</t>
-  </si>
-  <si>
-    <t>picture</t>
-  </si>
-  <si>
-    <t>user Name</t>
-  </si>
-  <si>
-    <t>Mary@gmail.com</t>
-  </si>
-  <si>
-    <t>********</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique </t>
-  </si>
-  <si>
-    <t>(forces unique screen names for all users by default)</t>
-  </si>
-  <si>
-    <t>UserName Table</t>
-  </si>
-  <si>
-    <t>check for availabliltiy user experience table</t>
-  </si>
-  <si>
-    <t>Hary</t>
-  </si>
-  <si>
-    <t>Lary</t>
   </si>
 </sst>
 </file>
@@ -569,7 +557,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,14 +624,6 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -747,7 +727,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="61">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -1402,23 +1382,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1769,21 +1737,8 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -2595,6 +2550,59 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5823D461-1651-46CD-AA63-CA13F4500146}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6029325" y="1600200"/>
+          <a:ext cx="3067050" cy="57150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>26</xdr:row>
@@ -2939,112 +2947,6 @@
         <a:xfrm>
           <a:off x="1905000" y="2314575"/>
           <a:ext cx="1752600" cy="3514725"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A96A671-13E6-431C-9DFF-2B157851322E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5848350" y="342900"/>
-          <a:ext cx="3695700" cy="314325"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F6309D6-1C2E-4A4B-8D2A-4C1C91736249}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5876925" y="419100"/>
-          <a:ext cx="3676650" cy="361950"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3392,80 +3294,80 @@
   <sheetData>
     <row r="1" spans="2:10" ht="21" x14ac:dyDescent="0.25">
       <c r="E1" s="80" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E2" s="18" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D4" s="128" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="E4" s="128" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F4" s="128" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D5" s="128" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="E5" s="128"/>
       <c r="F5" s="128" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="142"/>
       <c r="C6" s="143"/>
       <c r="D6" s="144" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E6" s="144" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F6" s="144" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="G6" s="144" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="H6" s="145" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="139" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C7" s="129" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D7" s="129" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E7" s="129" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F7" s="146" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="H7" s="137" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="140"/>
       <c r="C8" s="129" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D8" s="130"/>
       <c r="E8" s="130"/>
@@ -3486,19 +3388,19 @@
     </row>
     <row r="9" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="120" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C9" s="91" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D9" s="75" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E9" s="75" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F9" s="76" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G9" s="1">
         <v>44292</v>
@@ -3512,16 +3414,16 @@
     <row r="10" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="121"/>
       <c r="C10" s="77" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D10" s="78" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E10" s="78" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F10" s="79" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G10" s="1">
         <v>44292</v>
@@ -3535,16 +3437,16 @@
     <row r="11" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="122"/>
       <c r="C11" s="81" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D11" s="75" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="75" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F11" s="82" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G11" s="1">
         <v>44294</v>
@@ -3557,19 +3459,19 @@
     </row>
     <row r="12" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="123" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="83" t="s">
         <v>111</v>
-      </c>
-      <c r="C12" s="83" t="s">
-        <v>106</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F12" s="84" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="G12" s="1">
         <v>44296</v>
@@ -3583,16 +3485,16 @@
     <row r="13" spans="2:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="124"/>
       <c r="C13" s="85" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D13" s="86" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="86" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G13" s="1">
         <v>44299</v>
@@ -3606,10 +3508,10 @@
     <row r="14" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="125"/>
       <c r="C14" s="93" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D14" s="94" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E14" s="95"/>
       <c r="F14" s="96"/>
@@ -3625,16 +3527,16 @@
     <row r="15" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="126"/>
       <c r="C15" s="97" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F15" s="98" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G15" s="1">
         <v>44301</v>
@@ -3647,15 +3549,15 @@
     </row>
     <row r="16" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="126" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C16" s="99"/>
       <c r="D16" s="12"/>
       <c r="E16" s="19" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F16" s="100" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G16" s="1">
         <v>44301</v>
@@ -3669,16 +3571,16 @@
     <row r="17" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="126"/>
       <c r="C17" s="101" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F17" s="98" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G17" s="1">
         <v>44301</v>
@@ -3692,16 +3594,16 @@
     <row r="18" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="127"/>
       <c r="C18" s="102" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D18" s="103" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="103" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F18" s="104" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G18" s="1">
         <v>44301</v>
@@ -3717,7 +3619,7 @@
       <c r="C19" s="132"/>
       <c r="D19" s="133"/>
       <c r="E19" s="133" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F19" s="148"/>
       <c r="G19" s="1">
@@ -3734,7 +3636,7 @@
       <c r="C20" s="135"/>
       <c r="D20" s="136"/>
       <c r="E20" s="136" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F20" s="149"/>
       <c r="G20" s="150">
@@ -3799,8 +3701,8 @@
   </sheetPr>
   <dimension ref="C3:Q26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3897,14 +3799,14 @@
     <row r="8" spans="3:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="49"/>
       <c r="F8" s="17" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="I8" s="112" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="J8" s="115"/>
       <c r="K8" s="116" t="s">
@@ -3922,11 +3824,11 @@
     <row r="9" spans="3:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="49"/>
       <c r="F9" s="105" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="I9" s="106" t="s">
         <v>15</v>
@@ -3946,11 +3848,11 @@
       </c>
       <c r="D10" s="49"/>
       <c r="F10" s="105" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="I10" s="111" t="s">
         <v>47</v>
@@ -3962,7 +3864,7 @@
         <v>18</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N10" s="38" t="s">
         <v>33</v>
@@ -3976,7 +3878,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="19"/>
       <c r="H11" s="19" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="I11" s="109" t="s">
         <v>0</v>
@@ -4186,10 +4088,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="C1:Q38"/>
+  <dimension ref="C1:P38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4202,90 +4104,65 @@
     <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E2" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F3" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
+        <v>141</v>
+      </c>
+      <c r="O3" s="51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F4" s="65" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E2" s="59" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2" s="64" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="J2" t="s">
-        <v>170</v>
-      </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="F3" s="152" t="s">
-        <v>136</v>
-      </c>
-      <c r="G3" s="153" t="s">
-        <v>167</v>
-      </c>
-      <c r="I3" s="10" t="str">
-        <f>I2</f>
-        <v xml:space="preserve">Unique </v>
-      </c>
-      <c r="O3" s="154"/>
-      <c r="P3" s="155" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="F4" s="65" t="s">
-        <v>48</v>
-      </c>
       <c r="G4" t="s">
-        <v>168</v>
-      </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="156" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q4" s="157"/>
-    </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="O4" s="66"/>
+      <c r="P4" s="53"/>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E5" s="34"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="158" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q5" s="159"/>
-    </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="O6" s="12"/>
-      <c r="P6" s="158" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q6" s="159"/>
-    </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="O5" s="67"/>
+      <c r="P5" s="55"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="O6" s="67"/>
+      <c r="P6" s="55"/>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E7" s="58" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
-      </c>
-      <c r="O7" s="12"/>
-      <c r="P7" s="158"/>
-      <c r="Q7" s="159"/>
-    </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="O7" s="67"/>
+      <c r="P7" s="55"/>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F8" s="88" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G8" s="89"/>
       <c r="H8" s="60"/>
@@ -4294,53 +4171,54 @@
       <c r="K8" s="60"/>
       <c r="L8" s="60"/>
       <c r="M8" s="53"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="158"/>
-      <c r="Q8" s="159"/>
-    </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="O8" s="67"/>
+      <c r="P8" s="55"/>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F9" s="62" t="s">
-        <v>165</v>
-      </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+        <v>49</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="55"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="158"/>
-      <c r="Q9" s="159"/>
-    </row>
-    <row r="10" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O9" s="67"/>
+      <c r="P9" s="55"/>
+    </row>
+    <row r="10" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="62" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="55"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="158"/>
-      <c r="Q10" s="159"/>
-    </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="O10" s="67"/>
+      <c r="P10" s="55"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" s="118" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="F11" s="62" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -4348,70 +4226,66 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="55"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="158"/>
-      <c r="Q11" s="159"/>
-    </row>
-    <row r="12" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O11" s="68"/>
+      <c r="P11" s="57"/>
+    </row>
+    <row r="12" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="119" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="F12" s="62" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L12" s="12"/>
       <c r="M12" s="55"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="160"/>
-      <c r="Q12" s="161"/>
-    </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F13" s="62" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>63</v>
-      </c>
       <c r="I13" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="M13" s="55" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F14" s="62" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -4420,12 +4294,12 @@
       <c r="L14" s="12"/>
       <c r="M14" s="55"/>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F15" s="63" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G15" s="72" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H15" s="61"/>
       <c r="I15" s="61"/>
@@ -4439,16 +4313,16 @@
     </row>
     <row r="18" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E18" s="73" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F18" s="88" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G18" s="89"/>
     </row>
     <row r="19" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F19" s="52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G19" s="60">
         <v>20</v>
@@ -4457,41 +4331,41 @@
         <v>25</v>
       </c>
       <c r="I19" s="69" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F20" s="54" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I20" s="70" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F21" s="54" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="70" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F22" s="56" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G22" s="61"/>
       <c r="H22" s="61"/>
       <c r="I22" s="71" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="5:15" x14ac:dyDescent="0.25">
@@ -4499,53 +4373,53 @@
     </row>
     <row r="24" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E24" s="73" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F25" s="88" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G25" s="89"/>
       <c r="O25" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F26" s="66" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G26" s="60" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H26" s="60"/>
       <c r="I26" s="53"/>
       <c r="K26" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F27" s="67" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="55"/>
       <c r="O27" s="51" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F28" s="67" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="55"/>
       <c r="O28" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="5:15" x14ac:dyDescent="0.25">
@@ -4554,66 +4428,66 @@
       <c r="H29" s="61"/>
       <c r="I29" s="57"/>
       <c r="O29" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E31" s="74" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="F31" s="114" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G32" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G33" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="G34" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I34" s="90" t="b">
         <v>1</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.25">
@@ -4633,12 +4507,9 @@
       <c r="F38" s="37"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{B1515359-AAAB-4136-AEBA-714E44CCBA99}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="80" orientation="landscape" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4661,7 +4532,7 @@
         <v>30</v>
       </c>
       <c r="C1" s="92" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D1" s="92" t="s">
         <v>31</v>
@@ -4669,7 +4540,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -4692,10 +4563,10 @@
   <sheetData>
     <row r="3" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="4:7" x14ac:dyDescent="0.25">
@@ -4706,29 +4577,29 @@
         <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="G5" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G9" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
@@ -4739,17 +4610,17 @@
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="E11" t="str">
         <f>E5</f>
         <v>Read Bio</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>